<commit_message>
Working on data model
</commit_message>
<xml_diff>
--- a/design/CL-PFU data model.xlsx
+++ b/design/CL-PFU data model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/TestTargetsDB/design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37C39A0-8F9D-6242-9817-32272836A014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83227BC-7F85-CC4D-9B2E-4B9A2D20EB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{7D1B523B-6A41-0844-B2C9-E0154220E900}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="10" xr2:uid="{7D1B523B-6A41-0844-B2C9-E0154220E900}"/>
   </bookViews>
   <sheets>
     <sheet name="Ledger.side" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,11 @@
     <sheet name="ECC.stage" sheetId="4" r:id="rId5"/>
     <sheet name="IEAMW" sheetId="6" r:id="rId6"/>
     <sheet name="PSUT" sheetId="7" r:id="rId7"/>
-    <sheet name="ForeignKeys" sheetId="10" r:id="rId8"/>
+    <sheet name="Method" sheetId="15" r:id="rId8"/>
+    <sheet name="Industry" sheetId="12" r:id="rId9"/>
+    <sheet name="Product" sheetId="13" r:id="rId10"/>
+    <sheet name="CompletedAllocationTable" sheetId="14" r:id="rId11"/>
+    <sheet name="ForeignKeys" sheetId="10" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="322">
   <si>
     <t>Energy</t>
   </si>
@@ -148,13 +152,874 @@
   </si>
   <si>
     <t>ECC.stage</t>
+  </si>
+  <si>
+    <t>IndustryID</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Resources</t>
+  </si>
+  <si>
+    <t>Imports</t>
+  </si>
+  <si>
+    <t>International marine bunkers</t>
+  </si>
+  <si>
+    <t>International aviation bunkers</t>
+  </si>
+  <si>
+    <t>Stock changes</t>
+  </si>
+  <si>
+    <t>Transfers</t>
+  </si>
+  <si>
+    <t>Statistical differences</t>
+  </si>
+  <si>
+    <t>Manufacture</t>
+  </si>
+  <si>
+    <t>Main activity producer electricity plants</t>
+  </si>
+  <si>
+    <t>Autoproducer electricity plants</t>
+  </si>
+  <si>
+    <t>Main activity producer CHP plants</t>
+  </si>
+  <si>
+    <t>Autoproducer CHP plants</t>
+  </si>
+  <si>
+    <t>Main activity producer heat plants</t>
+  </si>
+  <si>
+    <t>Autoproducer heat plants</t>
+  </si>
+  <si>
+    <t>Heat pumps</t>
+  </si>
+  <si>
+    <t>Electric boilers</t>
+  </si>
+  <si>
+    <t>Chemical heat for electricity production</t>
+  </si>
+  <si>
+    <t>Blast furnaces</t>
+  </si>
+  <si>
+    <t>Gas works</t>
+  </si>
+  <si>
+    <t>Coke ovens</t>
+  </si>
+  <si>
+    <t>Patent fuel plants</t>
+  </si>
+  <si>
+    <t>BKB/peat briquette plants</t>
+  </si>
+  <si>
+    <t>Oil refineries</t>
+  </si>
+  <si>
+    <t>Petrochemical plants</t>
+  </si>
+  <si>
+    <t>Coal liquefaction plants</t>
+  </si>
+  <si>
+    <t>Gas-to-liquids (GTL) plants</t>
+  </si>
+  <si>
+    <t>For blended natural gas</t>
+  </si>
+  <si>
+    <t>Charcoal production plants</t>
+  </si>
+  <si>
+    <t>Non-specified (transformation)</t>
+  </si>
+  <si>
+    <t>Coal mines</t>
+  </si>
+  <si>
+    <t>Oil and gas extraction</t>
+  </si>
+  <si>
+    <t>Gasification plants for biogases</t>
+  </si>
+  <si>
+    <t>Liquefaction (LNG) / regasification plants</t>
+  </si>
+  <si>
+    <t>Own use in electricity, CHP and heat plants</t>
+  </si>
+  <si>
+    <t>Pumped storage plants</t>
+  </si>
+  <si>
+    <t>Nuclear industry</t>
+  </si>
+  <si>
+    <t>Non-specified (energy)</t>
+  </si>
+  <si>
+    <t>Losses</t>
+  </si>
+  <si>
+    <t>Mining and quarrying</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Iron and steel</t>
+  </si>
+  <si>
+    <t>Chemical and petrochemical</t>
+  </si>
+  <si>
+    <t>Non-ferrous metals</t>
+  </si>
+  <si>
+    <t>Non-metallic minerals</t>
+  </si>
+  <si>
+    <t>Transport equipment</t>
+  </si>
+  <si>
+    <t>Machinery</t>
+  </si>
+  <si>
+    <t>Food and tobacco</t>
+  </si>
+  <si>
+    <t>Paper, pulp and printing</t>
+  </si>
+  <si>
+    <t>Wood and wood products</t>
+  </si>
+  <si>
+    <t>Textile and leather</t>
+  </si>
+  <si>
+    <t>Industry not elsewhere specified</t>
+  </si>
+  <si>
+    <t>Domestic aviation</t>
+  </si>
+  <si>
+    <t>Road</t>
+  </si>
+  <si>
+    <t>Rail</t>
+  </si>
+  <si>
+    <t>Pipeline transport</t>
+  </si>
+  <si>
+    <t>Domestic navigation</t>
+  </si>
+  <si>
+    <t>Transport not elsewhere specified</t>
+  </si>
+  <si>
+    <t>International aviation</t>
+  </si>
+  <si>
+    <t>International navigation</t>
+  </si>
+  <si>
+    <t>Residential</t>
+  </si>
+  <si>
+    <t>Commercial and public services</t>
+  </si>
+  <si>
+    <t>Agriculture/forestry</t>
+  </si>
+  <si>
+    <t>Fishing</t>
+  </si>
+  <si>
+    <t>Final consumption not elsewhere specified</t>
+  </si>
+  <si>
+    <t>Non-energy use in construction</t>
+  </si>
+  <si>
+    <t>Non-energy use in mining and quarrying</t>
+  </si>
+  <si>
+    <t>Non-energy use in iron and steel</t>
+  </si>
+  <si>
+    <t>Non-energy use in chemical/petrochemical</t>
+  </si>
+  <si>
+    <t>Non-energy use in non-ferrous metals</t>
+  </si>
+  <si>
+    <t>Non-energy use in non-metallic minerals</t>
+  </si>
+  <si>
+    <t>Non-energy use in transport equipment</t>
+  </si>
+  <si>
+    <t>Non-energy use in machinery</t>
+  </si>
+  <si>
+    <t>Non-energy use in food/beverages/tobacco</t>
+  </si>
+  <si>
+    <t>Non-energy use in paper/pulp and printing</t>
+  </si>
+  <si>
+    <t>Non-energy use in wood and wood products</t>
+  </si>
+  <si>
+    <t>Non-energy use in textiles and leather</t>
+  </si>
+  <si>
+    <t>Non-energy use in industry not elsewhere specified</t>
+  </si>
+  <si>
+    <t>Non-energy use in other</t>
+  </si>
+  <si>
+    <t>Exports</t>
+  </si>
+  <si>
+    <t>Air compressors</t>
+  </si>
+  <si>
+    <t>Ammonia synthesizers</t>
+  </si>
+  <si>
+    <t>Bayer kilns</t>
+  </si>
+  <si>
+    <t>Blast oxygen furnaces</t>
+  </si>
+  <si>
+    <t>Bulk carrier ships</t>
+  </si>
+  <si>
+    <t>Charcoal stoves</t>
+  </si>
+  <si>
+    <t>Clinker kilns</t>
+  </si>
+  <si>
+    <t>Coal stoves</t>
+  </si>
+  <si>
+    <t>Commercial electric ovens</t>
+  </si>
+  <si>
+    <t>Commercial gas ovens</t>
+  </si>
+  <si>
+    <t>Commercial indoor electric lamps</t>
+  </si>
+  <si>
+    <t>Commercial outdoor electric lamps</t>
+  </si>
+  <si>
+    <t>Computers</t>
+  </si>
+  <si>
+    <t>Container ships</t>
+  </si>
+  <si>
+    <t>Diesel bulldozers</t>
+  </si>
+  <si>
+    <t>Diesel haulage trucks</t>
+  </si>
+  <si>
+    <t>Diesel HDVs</t>
+  </si>
+  <si>
+    <t>Diesel hydraulic mobiles</t>
+  </si>
+  <si>
+    <t>Diesel LDVs</t>
+  </si>
+  <si>
+    <t>Diesel pumps</t>
+  </si>
+  <si>
+    <t>Diesel rock borers</t>
+  </si>
+  <si>
+    <t>Diesel trains</t>
+  </si>
+  <si>
+    <t>Domestic aircraft</t>
+  </si>
+  <si>
+    <t>Domestic appliances</t>
+  </si>
+  <si>
+    <t>Domestic boats</t>
+  </si>
+  <si>
+    <t>Domestic electric lamps</t>
+  </si>
+  <si>
+    <t>Domestic electric ovens</t>
+  </si>
+  <si>
+    <t>Domestic fans</t>
+  </si>
+  <si>
+    <t>Domestic gas ovens</t>
+  </si>
+  <si>
+    <t>Electric arc furnaces</t>
+  </si>
+  <si>
+    <t>Electric cable cranes</t>
+  </si>
+  <si>
+    <t>Electric cable shovels</t>
+  </si>
+  <si>
+    <t>Electric cars</t>
+  </si>
+  <si>
+    <t>Electric continuous miners</t>
+  </si>
+  <si>
+    <t>Electric hand tools</t>
+  </si>
+  <si>
+    <t>Electric hydraulic mobiles</t>
+  </si>
+  <si>
+    <t>Electric pipeline gas compressors</t>
+  </si>
+  <si>
+    <t>Electric pumps</t>
+  </si>
+  <si>
+    <t>Electric space heaters</t>
+  </si>
+  <si>
+    <t>Electric trains</t>
+  </si>
+  <si>
+    <t>Electric water heaters</t>
+  </si>
+  <si>
+    <t>Electro chemical processors</t>
+  </si>
+  <si>
+    <t>Electrolytic smelters</t>
+  </si>
+  <si>
+    <t>Fishing vessels</t>
+  </si>
+  <si>
+    <t>Gas pump jacks</t>
+  </si>
+  <si>
+    <t>Gas space heaters</t>
+  </si>
+  <si>
+    <t>Gas water heaters</t>
+  </si>
+  <si>
+    <t>Gasoline LDVs</t>
+  </si>
+  <si>
+    <t>Gasoline motorcycles</t>
+  </si>
+  <si>
+    <t>General cargo ships</t>
+  </si>
+  <si>
+    <t>Heat machines</t>
+  </si>
+  <si>
+    <t>HVAC</t>
+  </si>
+  <si>
+    <t>Industrial electric lamps</t>
+  </si>
+  <si>
+    <t>Industrial electric process heaters</t>
+  </si>
+  <si>
+    <t>Industrial fans</t>
+  </si>
+  <si>
+    <t>Industrial refrigerators</t>
+  </si>
+  <si>
+    <t>International aircraft</t>
+  </si>
+  <si>
+    <t>Kerosene lamps</t>
+  </si>
+  <si>
+    <t>Kerosene stoves</t>
+  </si>
+  <si>
+    <t>LPG stoves</t>
+  </si>
+  <si>
+    <t>Machine tools</t>
+  </si>
+  <si>
+    <t>Material handlers</t>
+  </si>
+  <si>
+    <t>Natural gas pipeline gas compressors</t>
+  </si>
+  <si>
+    <t>Natural gas vehicles</t>
+  </si>
+  <si>
+    <t>Non-energy consumption</t>
+  </si>
+  <si>
+    <t>Oil lamps</t>
+  </si>
+  <si>
+    <t>Oil space heaters</t>
+  </si>
+  <si>
+    <t>Oil water heaters</t>
+  </si>
+  <si>
+    <t>Ore grinding mills</t>
+  </si>
+  <si>
+    <t>Paper machines</t>
+  </si>
+  <si>
+    <t>Refrigerators</t>
+  </si>
+  <si>
+    <t>Room air conditioners</t>
+  </si>
+  <si>
+    <t>Small scale biomass boilers</t>
+  </si>
+  <si>
+    <t>Solar thermal water heaters</t>
+  </si>
+  <si>
+    <t>Static diesel engines</t>
+  </si>
+  <si>
+    <t>Static gasoline engines</t>
+  </si>
+  <si>
+    <t>Steam boats</t>
+  </si>
+  <si>
+    <t>Steam cracking furnaces</t>
+  </si>
+  <si>
+    <t>Steam trains</t>
+  </si>
+  <si>
+    <t>Tanker ships</t>
+  </si>
+  <si>
+    <t>Televisions</t>
+  </si>
+  <si>
+    <t>Town gas lamps</t>
+  </si>
+  <si>
+    <t>Tractors</t>
+  </si>
+  <si>
+    <t>Wood stoves</t>
+  </si>
+  <si>
+    <t>ProductID</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Hard coal (if no detail)</t>
+  </si>
+  <si>
+    <t>Brown coal (if no detail)</t>
+  </si>
+  <si>
+    <t>Anthracite</t>
+  </si>
+  <si>
+    <t>Coking coal</t>
+  </si>
+  <si>
+    <t>Other bituminous coal</t>
+  </si>
+  <si>
+    <t>Sub-bituminous coal</t>
+  </si>
+  <si>
+    <t>Lignite</t>
+  </si>
+  <si>
+    <t>Patent fuel</t>
+  </si>
+  <si>
+    <t>Coke oven coke</t>
+  </si>
+  <si>
+    <t>Gas coke</t>
+  </si>
+  <si>
+    <t>Coal tar</t>
+  </si>
+  <si>
+    <t>BKB</t>
+  </si>
+  <si>
+    <t>Gas works gas</t>
+  </si>
+  <si>
+    <t>Coke oven gas</t>
+  </si>
+  <si>
+    <t>Blast furnace gas</t>
+  </si>
+  <si>
+    <t>Other recovered gases</t>
+  </si>
+  <si>
+    <t>Peat</t>
+  </si>
+  <si>
+    <t>Peat products</t>
+  </si>
+  <si>
+    <t>Oil shale and oil sands</t>
+  </si>
+  <si>
+    <t>Natural gas</t>
+  </si>
+  <si>
+    <t>Crude/NGL/feedstocks (if no detail)</t>
+  </si>
+  <si>
+    <t>Crude oil</t>
+  </si>
+  <si>
+    <t>Natural gas liquids</t>
+  </si>
+  <si>
+    <t>Refinery feedstocks</t>
+  </si>
+  <si>
+    <t>Additives/blending components</t>
+  </si>
+  <si>
+    <t>Other hydrocarbons</t>
+  </si>
+  <si>
+    <t>Refinery gas</t>
+  </si>
+  <si>
+    <t>Ethane</t>
+  </si>
+  <si>
+    <t>Liquefied petroleum gases (LPG)</t>
+  </si>
+  <si>
+    <t>Motor gasoline excl. biofuels</t>
+  </si>
+  <si>
+    <t>Aviation gasoline</t>
+  </si>
+  <si>
+    <t>Gasoline type jet fuel</t>
+  </si>
+  <si>
+    <t>Kerosene type jet fuel excl. biofuels</t>
+  </si>
+  <si>
+    <t>Other kerosene</t>
+  </si>
+  <si>
+    <t>Gas/diesel oil excl. biofuels</t>
+  </si>
+  <si>
+    <t>Fuel oil</t>
+  </si>
+  <si>
+    <t>Naphtha</t>
+  </si>
+  <si>
+    <t>White spirit &amp; SBP</t>
+  </si>
+  <si>
+    <t>Lubricants</t>
+  </si>
+  <si>
+    <t>Bitumen</t>
+  </si>
+  <si>
+    <t>Paraffin waxes</t>
+  </si>
+  <si>
+    <t>Petroleum coke</t>
+  </si>
+  <si>
+    <t>Other oil products</t>
+  </si>
+  <si>
+    <t>Industrial waste</t>
+  </si>
+  <si>
+    <t>Municipal waste (renewable)</t>
+  </si>
+  <si>
+    <t>Municipal waste (non-renewable)</t>
+  </si>
+  <si>
+    <t>Primary solid biofuels</t>
+  </si>
+  <si>
+    <t>Biogases</t>
+  </si>
+  <si>
+    <t>Biogasoline</t>
+  </si>
+  <si>
+    <t>Biodiesels</t>
+  </si>
+  <si>
+    <t>Bio jet kerosene</t>
+  </si>
+  <si>
+    <t>Other liquid biofuels</t>
+  </si>
+  <si>
+    <t>Non-specified primary biofuels and waste</t>
+  </si>
+  <si>
+    <t>Charcoal</t>
+  </si>
+  <si>
+    <t>Elec/heat output from non-specified manufactured gases</t>
+  </si>
+  <si>
+    <t>Heat output from non-specified combustible fuels</t>
+  </si>
+  <si>
+    <t>Nuclear</t>
+  </si>
+  <si>
+    <t>Hydro</t>
+  </si>
+  <si>
+    <t>Geothermal</t>
+  </si>
+  <si>
+    <t>Solar photovoltaics</t>
+  </si>
+  <si>
+    <t>Solar thermal</t>
+  </si>
+  <si>
+    <t>Tide, wave and ocean</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>Other sources</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Heat</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Feed</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>MacW</t>
+  </si>
+  <si>
+    <t>MF</t>
+  </si>
+  <si>
+    <t>KE</t>
+  </si>
+  <si>
+    <t>AirP</t>
+  </si>
+  <si>
+    <t>RaP</t>
+  </si>
+  <si>
+    <t>RoP</t>
+  </si>
+  <si>
+    <t>MaP</t>
+  </si>
+  <si>
+    <t>HPA</t>
+  </si>
+  <si>
+    <t>HPL</t>
+  </si>
+  <si>
+    <t>HPNG</t>
+  </si>
+  <si>
+    <t>HTH.1600.C</t>
+  </si>
+  <si>
+    <t>HTH.1300.C</t>
+  </si>
+  <si>
+    <t>HTH.1000.C</t>
+  </si>
+  <si>
+    <t>HTH.960.C</t>
+  </si>
+  <si>
+    <t>HTH.850.C</t>
+  </si>
+  <si>
+    <t>HTH.600.C</t>
+  </si>
+  <si>
+    <t>HTH.400.C</t>
+  </si>
+  <si>
+    <t>MTH.300.C</t>
+  </si>
+  <si>
+    <t>MTH.200.C</t>
+  </si>
+  <si>
+    <t>MTH.100.C</t>
+  </si>
+  <si>
+    <t>LTH.60.C</t>
+  </si>
+  <si>
+    <t>LTH.50.C</t>
+  </si>
+  <si>
+    <t>LTH.20.C</t>
+  </si>
+  <si>
+    <t>LTC.20.C</t>
+  </si>
+  <si>
+    <t>LTC.-10.C</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>AMW</t>
+  </si>
+  <si>
+    <t>HMW</t>
+  </si>
+  <si>
+    <t>NEU</t>
+  </si>
+  <si>
+    <t>CompletedAllocationTableID</t>
+  </si>
+  <si>
+    <t>MethodID</t>
+  </si>
+  <si>
+    <t>EfProduct</t>
+  </si>
+  <si>
+    <t>Machine</t>
+  </si>
+  <si>
+    <t>EuProduct</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>C1 [%]</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>PCM</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Final is primary</t>
+  </si>
+  <si>
+    <t>RCM</t>
+  </si>
+  <si>
+    <t>Primary energy as found in nature</t>
+  </si>
+  <si>
+    <t>PSM</t>
+  </si>
+  <si>
+    <t>Coal equivalent</t>
+  </si>
+  <si>
+    <t>Flow.aggregation.point</t>
+  </si>
+  <si>
+    <t>CompletedAllocationTable</t>
+  </si>
+  <si>
+    <t>C_source</t>
+  </si>
+  <si>
+    <t>WRLD</t>
+  </si>
+  <si>
+    <t>Liquified petroleum gas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -165,6 +1030,17 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -202,7 +1078,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -211,6 +1087,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -534,6 +1422,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -561,6 +1452,1226 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A192F7-E930-C04D-8F26-5B715BCE6631}">
+  <dimension ref="A1:B100"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="10">
+        <v>11</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="10">
+        <v>12</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
+        <v>13</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="10">
+        <v>14</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="10">
+        <v>15</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="10">
+        <v>16</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="10">
+        <v>17</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>18</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="10">
+        <v>19</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="10">
+        <v>20</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="10">
+        <v>21</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="10">
+        <v>22</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="10">
+        <v>23</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="10">
+        <v>24</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="10">
+        <v>25</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="10">
+        <v>26</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="10">
+        <v>27</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="10">
+        <v>28</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="10">
+        <v>29</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="10">
+        <v>30</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="10">
+        <v>31</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="10">
+        <v>32</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="10">
+        <v>33</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="10">
+        <v>34</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="10">
+        <v>35</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="10">
+        <v>36</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="10">
+        <v>37</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="10">
+        <v>38</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="10">
+        <v>39</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="10">
+        <v>40</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="10">
+        <v>41</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="10">
+        <v>42</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="10">
+        <v>43</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="10">
+        <v>44</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="10">
+        <v>45</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="10">
+        <v>46</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="10">
+        <v>47</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="10">
+        <v>48</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="10">
+        <v>49</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="10">
+        <v>50</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="10">
+        <v>51</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="10">
+        <v>52</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="10">
+        <v>53</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="10">
+        <v>54</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="10">
+        <v>55</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="10">
+        <v>56</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="10">
+        <v>57</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="10">
+        <v>58</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="10">
+        <v>59</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="10">
+        <v>60</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="10">
+        <v>61</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="10">
+        <v>62</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="10">
+        <v>63</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="10">
+        <v>64</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="10">
+        <v>65</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="10">
+        <v>66</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="10">
+        <v>67</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="10">
+        <v>68</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="10">
+        <v>69</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="10">
+        <v>70</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="10">
+        <v>71</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="10">
+        <v>72</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="10">
+        <v>73</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="10">
+        <v>74</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="10">
+        <v>75</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="10">
+        <v>76</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="10">
+        <v>77</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="10">
+        <v>78</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="10">
+        <v>79</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="10">
+        <v>80</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="10">
+        <v>81</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="10">
+        <v>82</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="10">
+        <v>83</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="10">
+        <v>84</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="10">
+        <v>85</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="10">
+        <v>86</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="10">
+        <v>87</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="10">
+        <v>88</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="10">
+        <v>89</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="10">
+        <v>90</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="10">
+        <v>91</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="10">
+        <v>92</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="10">
+        <v>93</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="10">
+        <v>94</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="10">
+        <v>95</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="10">
+        <v>96</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="10">
+        <v>97</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="10">
+        <v>98</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="10">
+        <v>99</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E00C8C8-73F6-8241-A54C-573B03BCB0F2}">
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="M2" s="6">
+        <v>2000</v>
+      </c>
+      <c r="N2" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E92DB7A8-D22B-8A49-BD6A-EB9C1CACC89E}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>309</v>
+      </c>
+      <c r="C4" t="s">
+        <v>309</v>
+      </c>
+      <c r="D4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>318</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>318</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>318</v>
+      </c>
+      <c r="B10" t="s">
+        <v>309</v>
+      </c>
+      <c r="C10" t="s">
+        <v>309</v>
+      </c>
+      <c r="D10" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>318</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>318</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>318</v>
+      </c>
+      <c r="B13" t="s">
+        <v>303</v>
+      </c>
+      <c r="C13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>318</v>
+      </c>
+      <c r="B14" t="s">
+        <v>304</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>318</v>
+      </c>
+      <c r="B15" t="s">
+        <v>305</v>
+      </c>
+      <c r="C15" t="s">
+        <v>201</v>
+      </c>
+      <c r="D15" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>318</v>
+      </c>
+      <c r="B16" t="s">
+        <v>306</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>318</v>
+      </c>
+      <c r="B17" t="s">
+        <v>319</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -17451,6 +19562,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -17485,7 +19599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D342CB12-39C5-CC45-9CCF-58CB02844BD4}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -17593,15 +19707,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{205D9C6A-F615-0B4F-93E1-B769B88F1995}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -17612,19 +19726,22 @@
         <v>27</v>
       </c>
       <c r="D1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -17635,15 +19752,18 @@
         <v>1960</v>
       </c>
       <c r="D2" t="s">
+        <v>310</v>
+      </c>
+      <c r="E2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>42</v>
       </c>
     </row>
@@ -17653,97 +19773,1420 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E92DB7A8-D22B-8A49-BD6A-EB9C1CACC89E}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD611AB-544F-9345-BB0A-B0EEB2332798}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>316</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42E131EA-01F7-4F4B-BE0F-A93429403C64}">
+  <dimension ref="A1:B168"/>
+  <sheetViews>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="A4" sqref="A3:A168"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="6">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B22" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B23" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="6">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B24" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B25" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B26" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
         <v>27</v>
       </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B28" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B29" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="6">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="6">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="6">
+        <v>31</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="6">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B33" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="6">
+        <v>33</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
         <v>34</v>
       </c>
-      <c r="D5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
+      <c r="B35" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="6">
+        <v>35</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="6">
+        <v>36</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="6">
+        <v>37</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="6">
+        <v>38</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="6">
+        <v>39</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="6">
+        <v>40</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="6">
+        <v>41</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="6">
+        <v>42</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="6">
+        <v>43</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="6">
+        <v>44</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="6">
+        <v>45</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="6">
+        <v>46</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="6">
+        <v>47</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="6">
+        <v>48</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="6">
+        <v>49</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="6">
+        <v>50</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="6">
+        <v>51</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="6">
+        <v>52</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="6">
+        <v>53</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="6">
+        <v>54</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="6">
+        <v>55</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="6">
+        <v>56</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="6">
+        <v>57</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="6">
+        <v>58</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="6">
+        <v>59</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="6">
+        <v>60</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="6">
+        <v>61</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="6">
+        <v>62</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="6">
+        <v>63</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="6">
+        <v>64</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="6">
+        <v>65</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="6">
+        <v>66</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="6">
+        <v>67</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="6">
+        <v>68</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="6">
+        <v>69</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="6">
+        <v>70</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="6">
+        <v>71</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="6">
+        <v>72</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="6">
+        <v>73</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="6">
+        <v>74</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="6">
+        <v>75</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="6">
+        <v>76</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="6">
+        <v>77</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="6">
+        <v>78</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="6">
+        <v>79</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="6">
+        <v>80</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="6">
+        <v>81</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="6">
+        <v>82</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="6">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="6">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="6">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="6">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="6">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="6">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="6">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="6">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="6">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="6">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="6">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="6">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="6">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="6">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="6">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="6">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="6">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="6">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="6">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="6">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="6">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="6">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="6">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="6">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="6">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="6">
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="6">
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="6">
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="6">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="6">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="6">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="6">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="6">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="6">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="6">
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="6">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="6">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="6">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="6">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="6">
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="6">
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="6">
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="6">
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="6">
+        <v>126</v>
+      </c>
+      <c r="B127" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="6">
+        <v>127</v>
+      </c>
+      <c r="B128" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="6">
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="6">
+        <v>129</v>
+      </c>
+      <c r="B130" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="6">
+        <v>130</v>
+      </c>
+      <c r="B131" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="6">
+        <v>131</v>
+      </c>
+      <c r="B132" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="6">
+        <v>132</v>
+      </c>
+      <c r="B133" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="6">
+        <v>133</v>
+      </c>
+      <c r="B134" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="6">
+        <v>134</v>
+      </c>
+      <c r="B135" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="6">
+        <v>135</v>
+      </c>
+      <c r="B136" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="6">
+        <v>136</v>
+      </c>
+      <c r="B137" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="6">
+        <v>137</v>
+      </c>
+      <c r="B138" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="6">
+        <v>138</v>
+      </c>
+      <c r="B139" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="6">
+        <v>139</v>
+      </c>
+      <c r="B140" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="6">
+        <v>140</v>
+      </c>
+      <c r="B141" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="6">
+        <v>141</v>
+      </c>
+      <c r="B142" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="6">
+        <v>142</v>
+      </c>
+      <c r="B143" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="6">
+        <v>143</v>
+      </c>
+      <c r="B144" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="6">
+        <v>144</v>
+      </c>
+      <c r="B145" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="6">
+        <v>145</v>
+      </c>
+      <c r="B146" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="6">
+        <v>146</v>
+      </c>
+      <c r="B147" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="6">
+        <v>147</v>
+      </c>
+      <c r="B148" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="6">
+        <v>148</v>
+      </c>
+      <c r="B149" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="6">
+        <v>149</v>
+      </c>
+      <c r="B150" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="6">
+        <v>150</v>
+      </c>
+      <c r="B151" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="6">
+        <v>151</v>
+      </c>
+      <c r="B152" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="6">
+        <v>152</v>
+      </c>
+      <c r="B153" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="6">
+        <v>153</v>
+      </c>
+      <c r="B154" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="6">
+        <v>154</v>
+      </c>
+      <c r="B155" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="6">
+        <v>155</v>
+      </c>
+      <c r="B156" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="6">
+        <v>156</v>
+      </c>
+      <c r="B157" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="6">
+        <v>157</v>
+      </c>
+      <c r="B158" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="6">
+        <v>158</v>
+      </c>
+      <c r="B159" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="6">
+        <v>159</v>
+      </c>
+      <c r="B160" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="6">
+        <v>160</v>
+      </c>
+      <c r="B161" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="6">
+        <v>161</v>
+      </c>
+      <c r="B162" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" s="6">
+        <v>162</v>
+      </c>
+      <c r="B163" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" s="6">
+        <v>163</v>
+      </c>
+      <c r="B164" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" s="6">
+        <v>164</v>
+      </c>
+      <c r="B165" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" s="6">
+        <v>165</v>
+      </c>
+      <c r="B166" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="6">
+        <v>166</v>
+      </c>
+      <c r="B167" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="6">
+        <v>167</v>
+      </c>
+      <c r="B168" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data model spreadsheet
</commit_message>
<xml_diff>
--- a/design/CL-PFU data model.xlsx
+++ b/design/CL-PFU data model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/TestTargetsDB/design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83227BC-7F85-CC4D-9B2E-4B9A2D20EB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D1D5AE-0E85-F74E-BBBD-DB96F6903AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="10" xr2:uid="{7D1B523B-6A41-0844-B2C9-E0154220E900}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="319">
   <si>
     <t>Energy</t>
   </si>
@@ -973,9 +973,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>C1 [%]</t>
-  </si>
-  <si>
     <t>Method</t>
   </si>
   <si>
@@ -1007,12 +1004,6 @@
   </si>
   <si>
     <t>C_source</t>
-  </si>
-  <si>
-    <t>WRLD</t>
-  </si>
-  <si>
-    <t>Liquified petroleum gas</t>
   </si>
 </sst>
 </file>
@@ -2275,7 +2266,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2293,7 +2284,7 @@
         <v>15</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>28</v>
@@ -2305,7 +2296,7 @@
         <v>31</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>303</v>
@@ -2329,55 +2320,25 @@
         <v>19</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="M2" s="6">
-        <v>2000</v>
-      </c>
-      <c r="N2" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>320</v>
-      </c>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
@@ -2415,6 +2376,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2423,7 +2385,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A17"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2478,10 +2440,10 @@
         <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D4" t="s">
         <v>302</v>
@@ -2531,7 +2493,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
@@ -2545,7 +2507,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
@@ -2559,13 +2521,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D10" t="s">
         <v>302</v>
@@ -2573,7 +2535,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
@@ -2587,7 +2549,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B12" t="s">
         <v>31</v>
@@ -2601,7 +2563,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B13" t="s">
         <v>303</v>
@@ -2615,7 +2577,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B14" t="s">
         <v>304</v>
@@ -2629,7 +2591,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B15" t="s">
         <v>305</v>
@@ -2643,7 +2605,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B16" t="s">
         <v>306</v>
@@ -2657,10 +2619,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>317</v>
+      </c>
+      <c r="B17" t="s">
         <v>318</v>
-      </c>
-      <c r="B17" t="s">
-        <v>319</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
@@ -19726,7 +19688,7 @@
         <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E1" t="s">
         <v>28</v>
@@ -19752,7 +19714,7 @@
         <v>1960</v>
       </c>
       <c r="D2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -19787,10 +19749,10 @@
         <v>302</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -19798,10 +19760,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -19809,10 +19771,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>313</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -19820,10 +19782,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>315</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>